<commit_message>
feat: dto and middleware
</commit_message>
<xml_diff>
--- a/Contacts_Properties.xlsx
+++ b/Contacts_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Amwhiz Projects\Personal\hubspot_properties_migration\proprties_migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1ADF32-8F79-494E-BB10-7D0636B14FEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE6031E-DC48-424C-82DA-B06F93E35C60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Object Type</t>
   </si>
@@ -70,9 +70,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Sports, Music, Reading</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>Birthday1</t>
+  </si>
+  <si>
+    <t>Sports, Music, Reading, Writing</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -558,10 +558,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -581,10 +581,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -604,10 +604,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -616,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -627,13 +627,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -650,13 +650,13 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -673,13 +673,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -696,13 +696,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -719,13 +719,13 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -737,7 +737,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 A9:B9 A2:B2 E2:G2 A3:B3 E3:G3 A4:B4 E4:G4 A5:B5 E5:G5 A6:B6 E6:G6 A7:B7 E7:G7 A8:B8 E8:G8 E9:G9" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 A9:B9 A2:B2 E2:G2 A3:B3 E3:G3 A4:B4 E4:F4 A5:B5 E5:G5 A6:B6 E6:G6 A7:B7 E7:G7 A8:B8 E8:G8 E9:G9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>